<commit_message>
new topic for java
</commit_message>
<xml_diff>
--- a/topics.xlsx
+++ b/topics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="161">
   <si>
     <t xml:space="preserve">Topic Level</t>
   </si>
@@ -49,81 +49,114 @@
     <t xml:space="preserve">Collections &amp; Generics</t>
   </si>
   <si>
+    <t xml:space="preserve">DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core framework for data structures like List, Set, and Map; understanding performance trade-offs is crucial for writing efficient code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-27 12:03:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generics and Type Safety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides stronger type checks at compile time and reduces runtime errors, enabling reusable and flexible code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-27 12:10:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Executor Framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multithreading &amp; Concurrency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simplifies thread management and improves scalability by abstracting low-level thread creation and pooling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-27 12:17:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synchronization &amp; Locks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essential for handling shared resources safely in multi-threaded applications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-27 13:08:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lambda Expressions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functional Programming &amp; Java 8+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduces functional style programming, reducing boilerplate code and improving readability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-27 13:28:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Streams API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides powerful data processing pipelines with filtering, mapping, and reducing operations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-27 13:38:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional &amp; Null Safety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helps developers write safer code by avoiding NullPointerExceptions and encouraging explicit handling of missing values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-27 13:52:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Testing with JUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing &amp; Debugging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fundamental for verifying application correctness and maintaining quality over time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-27 13:56:49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logging (SLF4J, Logback)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical for debugging, monitoring, and troubleshooting applications in production.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-27 14:19:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maven Basics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widely used build automation tool for managing dependencies and project lifecycles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-27 14:22:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gradle Basics</t>
+  </si>
+  <si>
     <t xml:space="preserve">NEW</t>
   </si>
   <si>
-    <t xml:space="preserve">Core framework for data structures like List, Set, and Map; understanding performance trade-offs is crucial for writing efficient code.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generics and Type Safety</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provides stronger type checks at compile time and reduces runtime errors, enabling reusable and flexible code.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Executor Framework</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multithreading &amp; Concurrency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simplifies thread management and improves scalability by abstracting low-level thread creation and pooling.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synchronization &amp; Locks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Essential for handling shared resources safely in multi-threaded applications.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lambda Expressions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional Programming &amp; Java 8+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduces functional style programming, reducing boilerplate code and improving readability.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Streams API</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provides powerful data processing pipelines with filtering, mapping, and reducing operations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional &amp; Null Safety</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Helps developers write safer code by avoiding NullPointerExceptions and encouraging explicit handling of missing values.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit Testing with JUnit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing &amp; Debugging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fundamental for verifying application correctness and maintaining quality over time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logging (SLF4J, Logback)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Critical for debugging, monitoring, and troubleshooting applications in production.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maven Basics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Build Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Widely used build automation tool for managing dependencies and project lifecycles.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gradle Basics</t>
-  </si>
-  <si>
     <t xml:space="preserve">Flexible build tool offering faster builds and advanced dependency management compared to Maven.</t>
   </si>
   <si>
@@ -262,37 +295,214 @@
     <t xml:space="preserve">Automates build, test, and deployment pipelines, enabling continuous delivery.</t>
   </si>
   <si>
-    <t>DONE</t>
-  </si>
-  <si>
-    <t>2025-08-27 12:03:33</t>
-  </si>
-  <si>
-    <t>2025-08-27 12:10:09</t>
-  </si>
-  <si>
-    <t>2025-08-27 12:17:53</t>
-  </si>
-  <si>
-    <t>2025-08-27 13:08:50</t>
-  </si>
-  <si>
-    <t>2025-08-27 13:28:36</t>
-  </si>
-  <si>
-    <t>2025-08-27 13:38:01</t>
-  </si>
-  <si>
-    <t>2025-08-27 13:52:18</t>
-  </si>
-  <si>
-    <t>2025-08-27 13:56:49</t>
-  </si>
-  <si>
-    <t>2025-08-27 14:19:08</t>
-  </si>
-  <si>
-    <t>2025-08-27 14:22:22</t>
+    <t xml:space="preserve">Java Modules (JPMS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modular programming introduced in Java 9; improves encapsulation and maintainability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annotations &amp; Reflection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runtime inspection and metadata-driven programming used in frameworks like Spring and Hibernate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serialization &amp; Deserialization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Techniques and pitfalls for converting objects to byte streams and back; includes security concerns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Records &amp; Sealed Classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modern Java features for immutable data carriers and controlled inheritance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern Matching (switch, instanceof)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improves readability and conciseness with new syntax for branching and type checks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fork/Join Framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concurrency &amp; Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efficient parallel execution framework for CPU-intensive tasks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ThreadLocal &amp; Concurrency Utilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced concurrency APIs: CountDownLatch, Semaphore, Phaser, ThreadLocal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disruptor Pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High-performance, low-latency concurrent programming pattern used in financial trading systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Data JPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simplifies data access by abstracting JPA/Hibernate and providing repository support.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides authentication, authorization, and integration with OAuth2/JWT.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring Batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enables scalable batch processing for enterprise applications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quarkus / Micronaut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternative frameworks optimized for microservices and cloud-native applications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDBC Deep Dive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Databases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covers connection pooling, transactions, and direct SQL performance optimization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoSQL Integration (MongoDB, Redis)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Techniques for integrating Java apps with NoSQL data stores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caching Frameworks (Ehcache, Redis, Caffeine)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improves performance through caching strategies and frameworks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mockito &amp; Testcontainers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powerful mocking and containerized integration testing frameworks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property-based Testing (jqwik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generates randomized test cases to discover edge conditions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static Analysis Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tools like SonarQube, Checkstyle, and SpotBugs for automated code quality checks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gradle Advanced (Kotlin DSL, Multi-module)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced Gradle usage with Kotlin DSL and multi-project builds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observability (Micrometer, OpenTelemetry)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud &amp; Monitoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metrics, tracing, and monitoring tools for distributed Java applications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Platforms (AWS/GCP/Azure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud &amp; Deployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deploying and managing Java applications on major cloud platforms.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service Mesh (Istio, Linkerd)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enhances microservice communication with traffic management and security.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domain-Driven Design (DDD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Architecture &amp; Patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strategic design concepts: aggregates, repositories, and bounded contexts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event-Driven Architecture (Kafka, RabbitMQ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Building resilient, asynchronous systems with messaging brokers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexagonal / Clean Architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design style separating business logic from infrastructure (ports &amp; adapters).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CQRS &amp; Event Sourcing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Separates read/write concerns and enables event replayability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JavaFX / Swing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frameworks for creating rich client desktop applications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REST &amp; GraphQL APIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design and implement APIs with Spring MVC/WebFlux and GraphQL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gRPC &amp; Protobuf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efficient, strongly typed communication between microservices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java &amp; AI/ML Integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI &amp; ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interfacing Java with machine learning libraries (Deeplearning4j, TensorFlow).</t>
   </si>
 </sst>
 </file>
@@ -393,16 +603,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32:F61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -435,13 +645,13 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s" s="0">
-        <v>81</v>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,7 +659,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -458,13 +668,13 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>82</v>
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,22 +682,22 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>83</v>
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,22 +705,22 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>84</v>
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -518,22 +728,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>85</v>
+        <v>24</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,22 +751,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>86</v>
+        <v>27</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,22 +774,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>87</v>
+        <v>30</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,22 +797,22 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" t="s" s="0">
-        <v>88</v>
+        <v>34</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,22 +820,22 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>89</v>
+        <v>37</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,22 +843,22 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" t="s" s="0">
-        <v>90</v>
+        <v>41</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,19 +866,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,19 +886,19 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,359 +906,959 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>